<commit_message>
draft use case diagram for coursework mannagement
</commit_message>
<xml_diff>
--- a/Project TimeTable.xlsx
+++ b/Project TimeTable.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cedric/Documents/finalproject/HEATSummerProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACC12E6-3244-EA42-B636-79C5FD6BDD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383E13C1-B8A1-344B-926A-6CB1185E0E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16560" xr2:uid="{6319CB8D-D377-A642-86B8-13A250C5DC4F}"/>
+    <workbookView xWindow="7040" yWindow="1300" windowWidth="27640" windowHeight="16560" xr2:uid="{6319CB8D-D377-A642-86B8-13A250C5DC4F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Timetable" sheetId="1" r:id="rId1"/>
+    <sheet name="Potential Licsencing Tools" sheetId="2" r:id="rId1"/>
+    <sheet name="Timetable" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="107">
   <si>
     <t>Hand In Report</t>
   </si>
@@ -253,12 +254,136 @@
   <si>
     <t xml:space="preserve">Finalise the application </t>
   </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Usage Extent</t>
+  </si>
+  <si>
+    <t>Funding</t>
+  </si>
+  <si>
+    <t>Standard (staff) Windows desktop</t>
+  </si>
+  <si>
+    <t>Open Access</t>
+  </si>
+  <si>
+    <t>Staff Remote Desktop</t>
+  </si>
+  <si>
+    <t>Student Remote Desktop</t>
+  </si>
+  <si>
+    <t>Lecture Theatres</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>BYOD Staff</t>
+  </si>
+  <si>
+    <t>BYOD Students</t>
+  </si>
+  <si>
+    <t>Licensed Users</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>.net</t>
+  </si>
+  <si>
+    <t>jetBrains</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>framework</t>
+  </si>
+  <si>
+    <t>IDE</t>
+  </si>
+  <si>
+    <t>Latex</t>
+  </si>
+  <si>
+    <t>Editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	
+Microsoft Office</t>
+  </si>
+  <si>
+    <t>Office Tools</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Programming Language</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>QuickTime</t>
+  </si>
+  <si>
+    <t>Rstudio</t>
+  </si>
+  <si>
+    <t>Skype</t>
+  </si>
+  <si>
+    <t>Meeting tools</t>
+  </si>
+  <si>
+    <t>Timetabling</t>
+  </si>
+  <si>
+    <t>Syllabus Plus</t>
+  </si>
+  <si>
+    <t>Tableau</t>
+  </si>
+  <si>
+    <t>Data Analysis and Graphing</t>
+  </si>
+  <si>
+    <t>Texmaker</t>
+  </si>
+  <si>
+    <t>LaTex pdf viewer</t>
+  </si>
+  <si>
+    <t>Unitity</t>
+  </si>
+  <si>
+    <t>Game Engine</t>
+  </si>
+  <si>
+    <t>Visual Studio Code</t>
+  </si>
+  <si>
+    <t>Code Editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visual Studio </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,6 +444,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -552,7 +690,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -625,60 +763,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -696,9 +780,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -710,11 +791,86 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -722,23 +878,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1053,10 +1202,207 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9624F0-BA00-3C47-9062-76C5C69CC119}">
+  <dimension ref="A1:O16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.5" style="67" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="67" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="65" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="65" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="65" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.6640625" style="65" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="65" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.83203125" style="65" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36" style="65" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" style="65" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" style="65" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" style="65" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" style="65" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.83203125" style="65" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" style="65" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="65"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="66" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="66" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="66" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="66" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="66" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="66" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="67" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="67" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="67" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="67" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="67" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="67" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="69" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="67" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="67" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="67" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="67" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="67" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="67" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="67" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="67" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="67" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF3E7EED-3B8C-2940-B596-13E288946EC2}">
   <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -1082,165 +1428,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="35" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="28" t="s">
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="28" t="s">
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="30"/>
-    </row>
-    <row r="2" spans="1:28" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="54" t="s">
+      <c r="P1" s="44"/>
+    </row>
+    <row r="2" spans="1:28" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="F2" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="52" t="s">
+      <c r="I2" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="52" t="s">
+      <c r="J2" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="K2" s="52" t="s">
+      <c r="K2" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="L2" s="52" t="s">
+      <c r="L2" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="52" t="s">
+      <c r="M2" s="33" t="s">
         <v>55</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="O2" s="41" t="s">
+      <c r="O2" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="P2" s="42"/>
-    </row>
-    <row r="3" spans="1:28" s="64" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="56" t="s">
+      <c r="P2" s="46"/>
+    </row>
+    <row r="3" spans="1:28" s="41" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="59" t="s">
+      <c r="C3" s="64"/>
+      <c r="D3" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60" t="s">
+      <c r="E3" s="55"/>
+      <c r="F3" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="59" t="s">
+      <c r="G3" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="59"/>
-      <c r="I3" s="61" t="s">
+      <c r="H3" s="55"/>
+      <c r="I3" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="55" t="s">
+      <c r="J3" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="K3" s="59"/>
-      <c r="L3" s="62" t="s">
+      <c r="K3" s="55"/>
+      <c r="L3" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="M3" s="62" t="s">
+      <c r="M3" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="N3" s="62" t="s">
+      <c r="N3" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="O3" s="60" t="s">
+      <c r="O3" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="63" t="s">
+      <c r="P3" s="40" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-    </row>
-    <row r="5" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="I5" s="49"/>
-    </row>
-    <row r="6" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="I6" s="49"/>
-    </row>
-    <row r="7" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="I7" s="49"/>
-    </row>
-    <row r="8" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="I8" s="49"/>
-    </row>
-    <row r="9" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="I9" s="49"/>
+    <row r="4" spans="1:28" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="1:28" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="31"/>
+    </row>
+    <row r="6" spans="1:28" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I6" s="31"/>
+    </row>
+    <row r="7" spans="1:28" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="31"/>
+    </row>
+    <row r="8" spans="1:28" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="31"/>
+    </row>
+    <row r="9" spans="1:28" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="31"/>
     </row>
     <row r="10" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:28" s="22" customFormat="1" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="40"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="61"/>
       <c r="I11" s="23"/>
     </row>
     <row r="12" spans="1:28" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="53"/>
       <c r="I12" s="21"/>
     </row>
     <row r="13" spans="1:28" s="2" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1292,42 +1638,42 @@
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26" t="s">
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26" t="s">
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="26"/>
-      <c r="S16" s="26"/>
-      <c r="T16" s="26"/>
-      <c r="U16" s="26"/>
-      <c r="V16" s="26" t="s">
+      <c r="P16" s="48"/>
+      <c r="Q16" s="48"/>
+      <c r="R16" s="48"/>
+      <c r="S16" s="48"/>
+      <c r="T16" s="48"/>
+      <c r="U16" s="48"/>
+      <c r="V16" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="W16" s="26"/>
-      <c r="X16" s="26"/>
-      <c r="Y16" s="26"/>
-      <c r="Z16" s="26"/>
-      <c r="AA16" s="26"/>
-      <c r="AB16" s="26"/>
+      <c r="W16" s="48"/>
+      <c r="X16" s="48"/>
+      <c r="Y16" s="48"/>
+      <c r="Z16" s="48"/>
+      <c r="AA16" s="48"/>
+      <c r="AB16" s="48"/>
     </row>
     <row r="17" spans="1:28" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
@@ -1438,20 +1784,20 @@
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="34" t="s">
+      <c r="O18" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="34"/>
-      <c r="S18" s="34"/>
-      <c r="T18" s="34"/>
-      <c r="U18" s="34"/>
-      <c r="V18" s="34"/>
-      <c r="W18" s="34"/>
-      <c r="X18" s="34"/>
-      <c r="Y18" s="34"/>
-      <c r="Z18" s="34"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="49"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+      <c r="U18" s="49"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="49"/>
+      <c r="X18" s="49"/>
+      <c r="Y18" s="49"/>
+      <c r="Z18" s="49"/>
       <c r="AA18" s="3"/>
       <c r="AB18" s="3"/>
     </row>
@@ -1486,42 +1832,42 @@
       <c r="AB19" s="3"/>
     </row>
     <row r="20" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26" t="s">
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26" t="s">
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="26"/>
-      <c r="S20" s="26"/>
-      <c r="T20" s="26"/>
-      <c r="U20" s="26"/>
-      <c r="V20" s="26" t="s">
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="48"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="48"/>
+      <c r="V20" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="W20" s="26"/>
-      <c r="X20" s="26"/>
-      <c r="Y20" s="26"/>
-      <c r="Z20" s="26"/>
-      <c r="AA20" s="26"/>
-      <c r="AB20" s="26"/>
+      <c r="W20" s="48"/>
+      <c r="X20" s="48"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="48"/>
+      <c r="AA20" s="48"/>
+      <c r="AB20" s="48"/>
     </row>
     <row r="21" spans="1:28" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
@@ -1613,78 +1959,78 @@
       <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="27" t="s">
+      <c r="H22" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="O22" s="27" t="s">
+      <c r="I22" s="50"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="50"/>
+      <c r="O22" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="27"/>
-      <c r="S22" s="27"/>
+      <c r="P22" s="50"/>
+      <c r="Q22" s="50"/>
+      <c r="R22" s="50"/>
+      <c r="S22" s="50"/>
       <c r="V22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="X22" s="47" t="s">
+      <c r="X22" s="29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:28" s="44" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="O23" s="45"/>
-      <c r="P23" s="45"/>
-      <c r="Q23" s="46" t="s">
+    <row r="23" spans="1:28" s="26" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="R23" s="45"/>
-      <c r="S23" s="45"/>
+      <c r="R23" s="27"/>
+      <c r="S23" s="27"/>
     </row>
     <row r="24" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26" t="s">
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26" t="s">
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26" t="s">
+      <c r="P24" s="48"/>
+      <c r="Q24" s="48"/>
+      <c r="R24" s="48"/>
+      <c r="S24" s="48"/>
+      <c r="T24" s="48"/>
+      <c r="U24" s="48"/>
+      <c r="V24" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="W24" s="26"/>
-      <c r="X24" s="26"/>
-      <c r="Y24" s="26"/>
-      <c r="Z24" s="26"/>
-      <c r="AA24" s="26"/>
-      <c r="AB24" s="26"/>
+      <c r="W24" s="48"/>
+      <c r="X24" s="48"/>
+      <c r="Y24" s="48"/>
+      <c r="Z24" s="48"/>
+      <c r="AA24" s="48"/>
+      <c r="AB24" s="48"/>
     </row>
     <row r="25" spans="1:28" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
@@ -1776,43 +2122,43 @@
       <c r="A26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="H26" s="27" t="s">
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="H26" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50"/>
       <c r="O26" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:28" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:28" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26" t="s">
+      <c r="B28" s="48"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="48"/>
     </row>
     <row r="29" spans="1:28" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
@@ -1842,44 +2188,59 @@
       <c r="I29" s="3">
         <v>45174</v>
       </c>
-      <c r="J29" s="48">
+      <c r="J29" s="30">
         <v>45175</v>
       </c>
-      <c r="K29" s="48">
+      <c r="K29" s="30">
         <v>45176</v>
       </c>
-      <c r="L29" s="48">
+      <c r="L29" s="30">
         <v>45177</v>
       </c>
-      <c r="M29" s="48">
+      <c r="M29" s="30">
         <v>45178</v>
       </c>
-      <c r="N29" s="48">
+      <c r="N29" s="30">
         <v>45179</v>
       </c>
     </row>
     <row r="30" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="I30" s="46" t="s">
+      <c r="I30" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="J30" s="50" t="s">
+      <c r="J30" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="K30" s="50"/>
-      <c r="L30" s="50"/>
-      <c r="M30" s="50"/>
-      <c r="N30" s="50"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="42"/>
     </row>
     <row r="31" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I31" s="2"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="50"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="V20:AB20"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="H24:N24"/>
+    <mergeCell ref="O24:U24"/>
+    <mergeCell ref="H22:L22"/>
+    <mergeCell ref="O16:U16"/>
+    <mergeCell ref="H16:N16"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A16:G16"/>
     <mergeCell ref="J30:N31"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="O2:P2"/>
@@ -1896,21 +2257,6 @@
     <mergeCell ref="V16:AB16"/>
     <mergeCell ref="A20:G20"/>
     <mergeCell ref="V24:AB24"/>
-    <mergeCell ref="O16:U16"/>
-    <mergeCell ref="H16:N16"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="V20:AB20"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="H24:N24"/>
-    <mergeCell ref="O24:U24"/>
-    <mergeCell ref="H22:L22"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>